<commit_message>
(refactor): Change name of form in config, add missing rendering column in meta excel
</commit_message>
<xml_diff>
--- a/metadata_example.xlsx
+++ b/metadata_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelbontyes/Repos/GitHub/clinical-content-tools/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajalodora/clinical-content-tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30FCFBAA-B396-914A-8162-1AC24A559AAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0179AD61-39C3-E74F-9C7B-39EF11853D68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19320" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="33600" windowHeight="19320" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Registration Workflow" sheetId="1" state="hidden" r:id="rId1"/>
@@ -43,7 +43,7 @@
     <sheet name="Drugs" sheetId="28" state="hidden" r:id="rId28"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'F06-PHQ-9'!$A$2:$AN$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'F06-PHQ-9'!$A$2:$AO$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">OptionSets!$A$2:$AH$6</definedName>
   </definedNames>
   <calcPr calcId="191029" calcOnSave="0"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7142" uniqueCount="4658">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7154" uniqueCount="4661">
   <si>
     <t>Step</t>
   </si>
@@ -14053,6 +14053,15 @@
   </si>
   <si>
     <t>LECHE TERAPÉUTICA, F75, polvo, 400g</t>
+  </si>
+  <si>
+    <t>Rendering</t>
+  </si>
+  <si>
+    <t>radio</t>
+  </si>
+  <si>
+    <t>numeric</t>
   </si>
 </sst>
 </file>
@@ -14458,6 +14467,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -14467,7 +14477,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -41596,13 +41605,13 @@
     <tabColor rgb="FFFFC000"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AN13"/>
+  <dimension ref="A1:AO13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D24" sqref="D24"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -41612,58 +41621,58 @@
     <col min="3" max="3" width="6.33203125" style="36" customWidth="1"/>
     <col min="4" max="4" width="54.1640625" customWidth="1"/>
     <col min="5" max="5" width="31.33203125" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="16.33203125" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="9" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="7.33203125" style="36" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="28.5" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="22" style="3" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="22" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="15" max="15" width="17.6640625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="16" max="16" width="18.6640625" customWidth="1" collapsed="1"/>
-    <col min="17" max="21" width="18.6640625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="18.6640625" customWidth="1"/>
-    <col min="23" max="23" width="16.33203125" customWidth="1"/>
-    <col min="24" max="24" width="10.83203125" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="18.6640625" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="15.5" customWidth="1" outlineLevel="1"/>
-    <col min="27" max="27" width="9.5" customWidth="1" outlineLevel="1"/>
-    <col min="28" max="30" width="4.5" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="6.6640625" customWidth="1" outlineLevel="1"/>
-    <col min="32" max="32" width="45.6640625" customWidth="1" outlineLevel="1"/>
-    <col min="33" max="33" width="14.33203125" customWidth="1" outlineLevel="1"/>
-    <col min="34" max="35" width="18.6640625" customWidth="1" outlineLevel="1"/>
-    <col min="36" max="36" width="11" customWidth="1" outlineLevel="1"/>
-    <col min="37" max="37" width="19.5" customWidth="1"/>
-    <col min="38" max="38" width="18.6640625" customWidth="1"/>
-    <col min="39" max="39" width="45" customWidth="1"/>
-    <col min="40" max="40" width="18.6640625" customWidth="1"/>
+    <col min="6" max="7" width="16.33203125" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="9" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="7.33203125" style="36" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="28.5" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="22" style="3" customWidth="1" collapsed="1"/>
+    <col min="12" max="15" width="22" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="16" width="17.6640625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="18.6640625" customWidth="1" collapsed="1"/>
+    <col min="18" max="22" width="18.6640625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="23" max="23" width="18.6640625" customWidth="1"/>
+    <col min="24" max="24" width="16.33203125" customWidth="1"/>
+    <col min="25" max="25" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="18.6640625" customWidth="1" outlineLevel="1"/>
+    <col min="27" max="27" width="15.5" customWidth="1" outlineLevel="1"/>
+    <col min="28" max="28" width="9.5" customWidth="1" outlineLevel="1"/>
+    <col min="29" max="31" width="4.5" customWidth="1" outlineLevel="1"/>
+    <col min="32" max="32" width="6.6640625" customWidth="1" outlineLevel="1"/>
+    <col min="33" max="33" width="45.6640625" customWidth="1" outlineLevel="1"/>
+    <col min="34" max="34" width="14.33203125" customWidth="1" outlineLevel="1"/>
+    <col min="35" max="36" width="18.6640625" customWidth="1" outlineLevel="1"/>
+    <col min="37" max="37" width="11" customWidth="1" outlineLevel="1"/>
+    <col min="38" max="38" width="19.5" customWidth="1"/>
+    <col min="39" max="39" width="18.6640625" customWidth="1"/>
+    <col min="40" max="40" width="45" customWidth="1"/>
+    <col min="41" max="41" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J1" s="54" t="s">
+    <row r="1" spans="1:41" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K1" s="55" t="s">
         <v>229</v>
       </c>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="54" t="s">
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="55" t="s">
         <v>230</v>
       </c>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
-      <c r="S1" s="55"/>
-      <c r="T1" s="55"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
       <c r="U1" s="56"/>
-      <c r="V1" s="46"/>
-      <c r="W1" s="57" t="s">
+      <c r="V1" s="57"/>
+      <c r="W1" s="46"/>
+      <c r="X1" s="58" t="s">
         <v>231</v>
       </c>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="55"/>
-    </row>
-    <row r="2" spans="1:40" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Y1" s="56"/>
+      <c r="Z1" s="56"/>
+    </row>
+    <row r="2" spans="1:41" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>232</v>
       </c>
@@ -41683,109 +41692,112 @@
         <v>237</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>4658</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="H2" s="37" t="s">
+      <c r="I2" s="37" t="s">
         <v>239</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="J2" s="49" t="s">
+      <c r="K2" s="49" t="s">
         <v>241</v>
       </c>
-      <c r="K2" s="49" t="s">
+      <c r="L2" s="49" t="s">
         <v>242</v>
       </c>
-      <c r="L2" s="49" t="s">
+      <c r="M2" s="49" t="s">
         <v>243</v>
       </c>
-      <c r="M2" s="49" t="s">
+      <c r="N2" s="49" t="s">
         <v>244</v>
       </c>
-      <c r="N2" s="49" t="s">
+      <c r="O2" s="49" t="s">
         <v>245</v>
       </c>
-      <c r="O2" s="50" t="s">
+      <c r="P2" s="50" t="s">
         <v>246</v>
       </c>
-      <c r="P2" s="49" t="s">
+      <c r="Q2" s="49" t="s">
         <v>247</v>
       </c>
-      <c r="Q2" s="49" t="s">
+      <c r="R2" s="49" t="s">
         <v>248</v>
       </c>
-      <c r="R2" s="49" t="s">
+      <c r="S2" s="49" t="s">
         <v>249</v>
       </c>
-      <c r="S2" s="49" t="s">
+      <c r="T2" s="49" t="s">
         <v>250</v>
       </c>
-      <c r="T2" s="49" t="s">
+      <c r="U2" s="49" t="s">
         <v>251</v>
       </c>
-      <c r="U2" s="50" t="s">
+      <c r="V2" s="50" t="s">
         <v>252</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AG2" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="AG2" s="2" t="s">
+      <c r="AH2" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AI2" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AK2" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="AK2" s="2" t="s">
+      <c r="AL2" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="AL2" s="2" t="s">
+      <c r="AM2" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="AM2" s="2" t="s">
+      <c r="AN2" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="AN2" s="2" t="s">
+      <c r="AO2" s="2" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="3" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>272</v>
       </c>
@@ -41795,7 +41807,7 @@
       <c r="C3" s="53">
         <v>1</v>
       </c>
-      <c r="D3" s="59" t="s">
+      <c r="D3" s="54" t="s">
         <v>274</v>
       </c>
       <c r="E3" t="s">
@@ -41804,45 +41816,48 @@
       <c r="F3" t="s">
         <v>276</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" t="s">
+        <v>4659</v>
+      </c>
+      <c r="H3" s="30" t="s">
         <v>277</v>
       </c>
-      <c r="H3" s="38"/>
-      <c r="I3" t="s">
+      <c r="I3" s="38"/>
+      <c r="J3" t="s">
         <v>278</v>
       </c>
-      <c r="J3" s="40"/>
-      <c r="K3" s="51"/>
+      <c r="K3" s="40"/>
       <c r="L3" s="51"/>
       <c r="M3" s="51"/>
       <c r="N3" s="51"/>
-      <c r="O3" s="52"/>
-      <c r="P3" s="40"/>
-      <c r="Q3" s="51"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="52"/>
+      <c r="Q3" s="40"/>
       <c r="R3" s="51"/>
       <c r="S3" s="51"/>
       <c r="T3" s="51"/>
-      <c r="U3" s="52"/>
-      <c r="V3" t="str">
-        <f t="shared" ref="V3:V13" si="0">IF(OR(N3&lt;&gt;"", T3&lt;&gt;"", Y3&lt;&gt;""), "Found", "Missing")</f>
+      <c r="U3" s="51"/>
+      <c r="V3" s="52"/>
+      <c r="W3" t="str">
+        <f t="shared" ref="W3:W13" si="0">IF(OR(O3&lt;&gt;"", U3&lt;&gt;"", Z3&lt;&gt;""), "Found", "Missing")</f>
         <v>Missing</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>279</v>
       </c>
-      <c r="Y3" s="51"/>
-      <c r="AJ3" t="s">
+      <c r="Z3" s="51"/>
+      <c r="AK3" t="s">
         <v>280</v>
       </c>
-      <c r="AK3" t="s">
+      <c r="AL3" t="s">
         <v>281</v>
       </c>
-      <c r="AL3" t="s">
+      <c r="AM3" t="s">
         <v>282</v>
       </c>
-      <c r="AM3" s="30"/>
-    </row>
-    <row r="4" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AN3" s="30"/>
+    </row>
+    <row r="4" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>272</v>
       </c>
@@ -41853,7 +41868,7 @@
         <f t="shared" ref="C4:C13" ca="1" si="1">OFFSET(C4,-1,0)+IF(OR(D4="",D4=OFFSET(D4,-1,0)),0,1)</f>
         <v>2</v>
       </c>
-      <c r="D4" s="59" t="s">
+      <c r="D4" s="54" t="s">
         <v>283</v>
       </c>
       <c r="E4" t="s">
@@ -41862,45 +41877,48 @@
       <c r="F4" t="s">
         <v>285</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="G4" t="s">
+        <v>4659</v>
+      </c>
+      <c r="H4" s="30" t="s">
         <v>277</v>
       </c>
-      <c r="H4" s="38"/>
-      <c r="I4" t="s">
+      <c r="I4" s="38"/>
+      <c r="J4" t="s">
         <v>278</v>
       </c>
-      <c r="J4" s="40"/>
-      <c r="K4" s="51"/>
+      <c r="K4" s="40"/>
       <c r="L4" s="51"/>
       <c r="M4" s="51"/>
       <c r="N4" s="51"/>
-      <c r="O4" s="52"/>
-      <c r="P4" s="40"/>
-      <c r="Q4" s="51"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="52"/>
+      <c r="Q4" s="40"/>
       <c r="R4" s="51"/>
       <c r="S4" s="51"/>
       <c r="T4" s="51"/>
-      <c r="U4" s="52"/>
-      <c r="V4" t="str">
+      <c r="U4" s="51"/>
+      <c r="V4" s="52"/>
+      <c r="W4" t="str">
         <f t="shared" si="0"/>
         <v>Missing</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>279</v>
       </c>
-      <c r="Y4" s="51"/>
-      <c r="AJ4" t="s">
+      <c r="Z4" s="51"/>
+      <c r="AK4" t="s">
         <v>280</v>
       </c>
-      <c r="AK4" t="s">
+      <c r="AL4" t="s">
         <v>286</v>
       </c>
-      <c r="AL4" t="s">
+      <c r="AM4" t="s">
         <v>282</v>
       </c>
-      <c r="AM4" s="30"/>
-    </row>
-    <row r="5" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AN4" s="30"/>
+    </row>
+    <row r="5" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>272</v>
       </c>
@@ -41911,7 +41929,7 @@
         <f t="shared" ca="1" si="1"/>
         <v>3</v>
       </c>
-      <c r="D5" s="59" t="s">
+      <c r="D5" s="54" t="s">
         <v>287</v>
       </c>
       <c r="E5" t="s">
@@ -41920,45 +41938,48 @@
       <c r="F5" t="s">
         <v>289</v>
       </c>
-      <c r="G5" s="30" t="s">
+      <c r="G5" t="s">
+        <v>4659</v>
+      </c>
+      <c r="H5" s="30" t="s">
         <v>277</v>
       </c>
-      <c r="H5" s="38"/>
-      <c r="I5" t="s">
+      <c r="I5" s="38"/>
+      <c r="J5" t="s">
         <v>278</v>
       </c>
-      <c r="J5" s="40"/>
-      <c r="K5" s="51"/>
+      <c r="K5" s="40"/>
       <c r="L5" s="51"/>
       <c r="M5" s="51"/>
       <c r="N5" s="51"/>
-      <c r="O5" s="52"/>
-      <c r="P5" s="40"/>
-      <c r="Q5" s="51"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="52"/>
+      <c r="Q5" s="40"/>
       <c r="R5" s="51"/>
       <c r="S5" s="51"/>
       <c r="T5" s="51"/>
-      <c r="U5" s="52"/>
-      <c r="V5" t="str">
+      <c r="U5" s="51"/>
+      <c r="V5" s="52"/>
+      <c r="W5" t="str">
         <f t="shared" si="0"/>
         <v>Missing</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>279</v>
       </c>
-      <c r="Y5" s="51"/>
-      <c r="AJ5" t="s">
+      <c r="Z5" s="51"/>
+      <c r="AK5" t="s">
         <v>280</v>
       </c>
-      <c r="AK5" t="s">
+      <c r="AL5" t="s">
         <v>290</v>
       </c>
-      <c r="AL5" t="s">
+      <c r="AM5" t="s">
         <v>282</v>
       </c>
-      <c r="AM5" s="30"/>
-    </row>
-    <row r="6" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AN5" s="30"/>
+    </row>
+    <row r="6" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>272</v>
       </c>
@@ -41969,7 +41990,7 @@
         <f t="shared" ca="1" si="1"/>
         <v>4</v>
       </c>
-      <c r="D6" s="59" t="s">
+      <c r="D6" s="54" t="s">
         <v>291</v>
       </c>
       <c r="E6" t="s">
@@ -41978,45 +41999,48 @@
       <c r="F6" t="s">
         <v>292</v>
       </c>
-      <c r="G6" s="30" t="s">
+      <c r="G6" t="s">
+        <v>4659</v>
+      </c>
+      <c r="H6" s="30" t="s">
         <v>277</v>
       </c>
-      <c r="H6" s="38"/>
-      <c r="I6" t="s">
+      <c r="I6" s="38"/>
+      <c r="J6" t="s">
         <v>278</v>
       </c>
-      <c r="J6" s="40"/>
-      <c r="K6" s="51"/>
+      <c r="K6" s="40"/>
       <c r="L6" s="51"/>
       <c r="M6" s="51"/>
       <c r="N6" s="51"/>
-      <c r="O6" s="52"/>
-      <c r="P6" s="40"/>
-      <c r="Q6" s="51"/>
+      <c r="O6" s="51"/>
+      <c r="P6" s="52"/>
+      <c r="Q6" s="40"/>
       <c r="R6" s="51"/>
       <c r="S6" s="51"/>
       <c r="T6" s="51"/>
-      <c r="U6" s="52"/>
-      <c r="V6" t="str">
+      <c r="U6" s="51"/>
+      <c r="V6" s="52"/>
+      <c r="W6" t="str">
         <f t="shared" si="0"/>
         <v>Missing</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>279</v>
       </c>
-      <c r="Y6" s="51"/>
-      <c r="AJ6" t="s">
+      <c r="Z6" s="51"/>
+      <c r="AK6" t="s">
         <v>280</v>
       </c>
-      <c r="AK6" t="s">
+      <c r="AL6" t="s">
         <v>293</v>
       </c>
-      <c r="AL6" t="s">
+      <c r="AM6" t="s">
         <v>282</v>
       </c>
-      <c r="AM6" s="30"/>
-    </row>
-    <row r="7" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AN6" s="30"/>
+    </row>
+    <row r="7" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>272</v>
       </c>
@@ -42027,7 +42051,7 @@
         <f t="shared" ca="1" si="1"/>
         <v>5</v>
       </c>
-      <c r="D7" s="59" t="s">
+      <c r="D7" s="54" t="s">
         <v>294</v>
       </c>
       <c r="E7" t="s">
@@ -42036,45 +42060,48 @@
       <c r="F7" t="s">
         <v>296</v>
       </c>
-      <c r="G7" s="30" t="s">
+      <c r="G7" t="s">
+        <v>4659</v>
+      </c>
+      <c r="H7" s="30" t="s">
         <v>277</v>
       </c>
-      <c r="H7" s="38"/>
-      <c r="I7" t="s">
+      <c r="I7" s="38"/>
+      <c r="J7" t="s">
         <v>278</v>
       </c>
-      <c r="J7" s="40"/>
-      <c r="K7" s="51"/>
+      <c r="K7" s="40"/>
       <c r="L7" s="51"/>
       <c r="M7" s="51"/>
       <c r="N7" s="51"/>
-      <c r="O7" s="52"/>
-      <c r="P7" s="40"/>
-      <c r="Q7" s="51"/>
+      <c r="O7" s="51"/>
+      <c r="P7" s="52"/>
+      <c r="Q7" s="40"/>
       <c r="R7" s="51"/>
       <c r="S7" s="51"/>
       <c r="T7" s="51"/>
-      <c r="U7" s="52"/>
-      <c r="V7" t="str">
+      <c r="U7" s="51"/>
+      <c r="V7" s="52"/>
+      <c r="W7" t="str">
         <f t="shared" si="0"/>
         <v>Missing</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Y7" t="s">
         <v>279</v>
       </c>
-      <c r="Y7" s="51"/>
-      <c r="AJ7" t="s">
+      <c r="Z7" s="51"/>
+      <c r="AK7" t="s">
         <v>280</v>
       </c>
-      <c r="AK7" t="s">
+      <c r="AL7" t="s">
         <v>297</v>
       </c>
-      <c r="AL7" t="s">
+      <c r="AM7" t="s">
         <v>282</v>
       </c>
-      <c r="AM7" s="30"/>
-    </row>
-    <row r="8" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AN7" s="30"/>
+    </row>
+    <row r="8" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>272</v>
       </c>
@@ -42085,7 +42112,7 @@
         <f t="shared" ca="1" si="1"/>
         <v>6</v>
       </c>
-      <c r="D8" s="59" t="s">
+      <c r="D8" s="54" t="s">
         <v>298</v>
       </c>
       <c r="E8" t="s">
@@ -42094,45 +42121,48 @@
       <c r="F8" t="s">
         <v>300</v>
       </c>
-      <c r="G8" s="30" t="s">
+      <c r="G8" t="s">
+        <v>4659</v>
+      </c>
+      <c r="H8" s="30" t="s">
         <v>277</v>
       </c>
-      <c r="H8" s="38"/>
-      <c r="I8" t="s">
+      <c r="I8" s="38"/>
+      <c r="J8" t="s">
         <v>278</v>
       </c>
-      <c r="J8" s="40"/>
-      <c r="K8" s="51"/>
+      <c r="K8" s="40"/>
       <c r="L8" s="51"/>
       <c r="M8" s="51"/>
       <c r="N8" s="51"/>
-      <c r="O8" s="52"/>
-      <c r="P8" s="40"/>
-      <c r="Q8" s="51"/>
+      <c r="O8" s="51"/>
+      <c r="P8" s="52"/>
+      <c r="Q8" s="40"/>
       <c r="R8" s="51"/>
       <c r="S8" s="51"/>
       <c r="T8" s="51"/>
-      <c r="U8" s="52"/>
-      <c r="V8" t="str">
+      <c r="U8" s="51"/>
+      <c r="V8" s="52"/>
+      <c r="W8" t="str">
         <f t="shared" si="0"/>
         <v>Missing</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Y8" t="s">
         <v>279</v>
       </c>
-      <c r="Y8" s="51"/>
-      <c r="AJ8" t="s">
+      <c r="Z8" s="51"/>
+      <c r="AK8" t="s">
         <v>280</v>
       </c>
-      <c r="AK8" t="s">
+      <c r="AL8" t="s">
         <v>301</v>
       </c>
-      <c r="AL8" t="s">
+      <c r="AM8" t="s">
         <v>282</v>
       </c>
-      <c r="AM8" s="30"/>
-    </row>
-    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AN8" s="30"/>
+    </row>
+    <row r="9" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>272</v>
       </c>
@@ -42143,7 +42173,7 @@
         <f t="shared" ca="1" si="1"/>
         <v>7</v>
       </c>
-      <c r="D9" s="59" t="s">
+      <c r="D9" s="54" t="s">
         <v>302</v>
       </c>
       <c r="E9" t="s">
@@ -42152,45 +42182,48 @@
       <c r="F9" t="s">
         <v>304</v>
       </c>
-      <c r="G9" s="30" t="s">
+      <c r="G9" t="s">
+        <v>4659</v>
+      </c>
+      <c r="H9" s="30" t="s">
         <v>277</v>
       </c>
-      <c r="H9" s="38"/>
-      <c r="I9" t="s">
+      <c r="I9" s="38"/>
+      <c r="J9" t="s">
         <v>278</v>
       </c>
-      <c r="J9" s="40"/>
-      <c r="K9" s="51"/>
+      <c r="K9" s="40"/>
       <c r="L9" s="51"/>
       <c r="M9" s="51"/>
       <c r="N9" s="51"/>
-      <c r="O9" s="52"/>
-      <c r="P9" s="40"/>
-      <c r="Q9" s="51"/>
+      <c r="O9" s="51"/>
+      <c r="P9" s="52"/>
+      <c r="Q9" s="40"/>
       <c r="R9" s="51"/>
       <c r="S9" s="51"/>
       <c r="T9" s="51"/>
-      <c r="U9" s="52"/>
-      <c r="V9" t="str">
+      <c r="U9" s="51"/>
+      <c r="V9" s="52"/>
+      <c r="W9" t="str">
         <f t="shared" si="0"/>
         <v>Missing</v>
       </c>
-      <c r="X9" t="s">
+      <c r="Y9" t="s">
         <v>279</v>
       </c>
-      <c r="Y9" s="51"/>
-      <c r="AJ9" t="s">
+      <c r="Z9" s="51"/>
+      <c r="AK9" t="s">
         <v>280</v>
       </c>
-      <c r="AK9" t="s">
+      <c r="AL9" t="s">
         <v>305</v>
       </c>
-      <c r="AL9" t="s">
+      <c r="AM9" t="s">
         <v>282</v>
       </c>
-      <c r="AM9" s="30"/>
-    </row>
-    <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AN9" s="30"/>
+    </row>
+    <row r="10" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>272</v>
       </c>
@@ -42201,7 +42234,7 @@
         <f t="shared" ca="1" si="1"/>
         <v>8</v>
       </c>
-      <c r="D10" s="59" t="s">
+      <c r="D10" s="54" t="s">
         <v>306</v>
       </c>
       <c r="E10" t="s">
@@ -42210,45 +42243,48 @@
       <c r="F10" t="s">
         <v>308</v>
       </c>
-      <c r="G10" s="30" t="s">
+      <c r="G10" t="s">
+        <v>4659</v>
+      </c>
+      <c r="H10" s="30" t="s">
         <v>277</v>
       </c>
-      <c r="H10" s="38"/>
-      <c r="I10" t="s">
+      <c r="I10" s="38"/>
+      <c r="J10" t="s">
         <v>278</v>
       </c>
-      <c r="J10" s="40"/>
-      <c r="K10" s="51"/>
+      <c r="K10" s="40"/>
       <c r="L10" s="51"/>
       <c r="M10" s="51"/>
       <c r="N10" s="51"/>
-      <c r="O10" s="52"/>
-      <c r="P10" s="40"/>
-      <c r="Q10" s="51"/>
+      <c r="O10" s="51"/>
+      <c r="P10" s="52"/>
+      <c r="Q10" s="40"/>
       <c r="R10" s="51"/>
       <c r="S10" s="51"/>
       <c r="T10" s="51"/>
-      <c r="U10" s="52"/>
-      <c r="V10" t="str">
+      <c r="U10" s="51"/>
+      <c r="V10" s="52"/>
+      <c r="W10" t="str">
         <f t="shared" si="0"/>
         <v>Missing</v>
       </c>
-      <c r="X10" t="s">
+      <c r="Y10" t="s">
         <v>279</v>
       </c>
-      <c r="Y10" s="51"/>
-      <c r="AJ10" t="s">
+      <c r="Z10" s="51"/>
+      <c r="AK10" t="s">
         <v>280</v>
       </c>
-      <c r="AK10" t="s">
+      <c r="AL10" t="s">
         <v>309</v>
       </c>
-      <c r="AL10" t="s">
+      <c r="AM10" t="s">
         <v>282</v>
       </c>
-      <c r="AM10" s="30"/>
-    </row>
-    <row r="11" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AN10" s="30"/>
+    </row>
+    <row r="11" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>272</v>
       </c>
@@ -42259,7 +42295,7 @@
         <f t="shared" ca="1" si="1"/>
         <v>9</v>
       </c>
-      <c r="D11" s="59" t="s">
+      <c r="D11" s="54" t="s">
         <v>310</v>
       </c>
       <c r="E11" t="s">
@@ -42268,45 +42304,48 @@
       <c r="F11" t="s">
         <v>312</v>
       </c>
-      <c r="G11" s="30" t="s">
+      <c r="G11" t="s">
+        <v>4659</v>
+      </c>
+      <c r="H11" s="30" t="s">
         <v>277</v>
       </c>
-      <c r="H11" s="38"/>
-      <c r="I11" t="s">
+      <c r="I11" s="38"/>
+      <c r="J11" t="s">
         <v>278</v>
       </c>
-      <c r="J11" s="40"/>
-      <c r="K11" s="51"/>
+      <c r="K11" s="40"/>
       <c r="L11" s="51"/>
       <c r="M11" s="51"/>
       <c r="N11" s="51"/>
-      <c r="O11" s="52"/>
-      <c r="P11" s="40"/>
-      <c r="Q11" s="51"/>
+      <c r="O11" s="51"/>
+      <c r="P11" s="52"/>
+      <c r="Q11" s="40"/>
       <c r="R11" s="51"/>
       <c r="S11" s="51"/>
       <c r="T11" s="51"/>
-      <c r="U11" s="52"/>
-      <c r="V11" t="str">
+      <c r="U11" s="51"/>
+      <c r="V11" s="52"/>
+      <c r="W11" t="str">
         <f t="shared" si="0"/>
         <v>Missing</v>
       </c>
-      <c r="X11" t="s">
+      <c r="Y11" t="s">
         <v>279</v>
       </c>
-      <c r="Y11" s="51"/>
-      <c r="AJ11" t="s">
+      <c r="Z11" s="51"/>
+      <c r="AK11" t="s">
         <v>280</v>
       </c>
-      <c r="AK11" t="s">
+      <c r="AL11" t="s">
         <v>313</v>
       </c>
-      <c r="AL11" t="s">
+      <c r="AM11" t="s">
         <v>282</v>
       </c>
-      <c r="AM11" s="30"/>
-    </row>
-    <row r="12" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AN11" s="30"/>
+    </row>
+    <row r="12" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>272</v>
       </c>
@@ -42317,60 +42356,63 @@
         <f t="shared" ca="1" si="1"/>
         <v>10</v>
       </c>
-      <c r="D12" s="59" t="s">
+      <c r="D12" s="54" t="s">
         <v>314</v>
       </c>
       <c r="G12" t="s">
+        <v>4660</v>
+      </c>
+      <c r="H12" t="s">
         <v>315</v>
       </c>
-      <c r="H12" s="38"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="51"/>
+      <c r="I12" s="38"/>
+      <c r="K12" s="40"/>
       <c r="L12" s="51"/>
       <c r="M12" s="51"/>
       <c r="N12" s="51"/>
-      <c r="O12" s="52"/>
-      <c r="P12" s="40"/>
-      <c r="Q12" s="51"/>
+      <c r="O12" s="51"/>
+      <c r="P12" s="52"/>
+      <c r="Q12" s="40"/>
       <c r="R12" s="51"/>
       <c r="S12" s="51"/>
       <c r="T12" s="51"/>
-      <c r="U12" s="52"/>
-      <c r="V12" t="str">
+      <c r="U12" s="51"/>
+      <c r="V12" s="52"/>
+      <c r="W12" t="str">
         <f t="shared" si="0"/>
         <v>Missing</v>
       </c>
-      <c r="X12" t="s">
+      <c r="Y12" t="s">
         <v>279</v>
       </c>
-      <c r="Z12" t="s">
+      <c r="AA12" t="s">
         <v>316</v>
       </c>
-      <c r="AA12" s="30"/>
-      <c r="AC12">
+      <c r="AB12" s="30"/>
+      <c r="AD12">
         <v>0</v>
       </c>
-      <c r="AD12" s="39">
+      <c r="AE12" s="39">
         <v>27</v>
       </c>
-      <c r="AE12" t="s">
+      <c r="AF12" t="s">
         <v>317</v>
       </c>
-      <c r="AG12" s="30"/>
-      <c r="AJ12" t="s">
+      <c r="AH12" s="30"/>
+      <c r="AK12" t="s">
         <v>280</v>
       </c>
-      <c r="AK12" t="s">
+      <c r="AL12" t="s">
         <v>318</v>
       </c>
-      <c r="AL12" t="s">
+      <c r="AM12" t="s">
         <v>282</v>
       </c>
-      <c r="AM12" s="30" t="s">
+      <c r="AN12" s="30" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="13" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>272</v>
       </c>
@@ -42381,48 +42423,51 @@
         <f t="shared" ca="1" si="1"/>
         <v>11</v>
       </c>
-      <c r="D13" s="59" t="s">
+      <c r="D13" s="54" t="s">
         <v>320</v>
       </c>
-      <c r="G13" s="30" t="s">
+      <c r="G13" t="s">
+        <v>445</v>
+      </c>
+      <c r="H13" s="30" t="s">
         <v>277</v>
       </c>
-      <c r="H13" s="38"/>
-      <c r="I13" t="s">
+      <c r="I13" s="38"/>
+      <c r="J13" t="s">
         <v>320</v>
       </c>
-      <c r="J13" s="40"/>
-      <c r="K13" s="51"/>
+      <c r="K13" s="40"/>
       <c r="L13" s="51"/>
       <c r="M13" s="51"/>
       <c r="N13" s="51"/>
-      <c r="O13" s="52"/>
-      <c r="P13" s="40"/>
-      <c r="Q13" s="51"/>
+      <c r="O13" s="51"/>
+      <c r="P13" s="52"/>
+      <c r="Q13" s="40"/>
       <c r="R13" s="51"/>
       <c r="S13" s="51"/>
       <c r="T13" s="51"/>
-      <c r="U13" s="52"/>
-      <c r="V13" t="str">
+      <c r="U13" s="51"/>
+      <c r="V13" s="52"/>
+      <c r="W13" t="str">
         <f t="shared" si="0"/>
         <v>Missing</v>
       </c>
-      <c r="X13" t="s">
+      <c r="Y13" t="s">
         <v>279</v>
       </c>
-      <c r="Y13" s="51"/>
-      <c r="Z13" s="30"/>
+      <c r="Z13" s="51"/>
       <c r="AA13" s="30"/>
-      <c r="AG13" s="30"/>
+      <c r="AB13" s="30"/>
+      <c r="AH13" s="30"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:AN2" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
+  <autoFilter ref="A2:AO2" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <mergeCells count="3">
-    <mergeCell ref="P1:U1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="J1:O1"/>
+    <mergeCell ref="Q1:V1"/>
+    <mergeCell ref="X1:Z1"/>
+    <mergeCell ref="K1:P1"/>
   </mergeCells>
-  <conditionalFormatting sqref="V1:V1048576">
+  <conditionalFormatting sqref="W1:W1048576">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Missing"</formula>
     </cfRule>
@@ -42431,7 +42476,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X3:X13" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3:Y13" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -42488,22 +42533,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G1" s="54" t="s">
+      <c r="G1" s="55" t="s">
         <v>229</v>
       </c>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="54" t="s">
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="55" t="s">
         <v>230</v>
       </c>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="57"/>
       <c r="S1" s="46"/>
       <c r="T1" s="41" t="s">
         <v>231</v>
@@ -42627,7 +42672,7 @@
         <f t="shared" ref="D3:D6" ca="1" si="0">IF(OFFSET(A3,-1,0)&lt;&gt;A3,1,OFFSET(D3,-1,0)+1)</f>
         <v>1</v>
       </c>
-      <c r="E3" s="59" t="s">
+      <c r="E3" s="54" t="s">
         <v>326</v>
       </c>
       <c r="G3" s="40"/>
@@ -42660,7 +42705,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
-      <c r="E4" s="59" t="s">
+      <c r="E4" s="54" t="s">
         <v>330</v>
       </c>
       <c r="G4" s="40"/>
@@ -42693,7 +42738,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
-      <c r="E5" s="59" t="s">
+      <c r="E5" s="54" t="s">
         <v>333</v>
       </c>
       <c r="G5" s="40"/>
@@ -42726,7 +42771,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>4</v>
       </c>
-      <c r="E6" s="59" t="s">
+      <c r="E6" s="54" t="s">
         <v>336</v>
       </c>
       <c r="G6" s="40"/>

</xml_diff>

<commit_message>
(feat) Add support for API-based calculations using concept IDs
</commit_message>
<xml_diff>
--- a/metadata_example.xlsx
+++ b/metadata_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajalodora/clinical-content-tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0179AD61-39C3-E74F-9C7B-39EF11853D68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14BC38EA-7550-3B48-B1DA-75F007BC5D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="33600" windowHeight="19320" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2400" yWindow="1700" windowWidth="33600" windowHeight="19320" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Registration Workflow" sheetId="1" state="hidden" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7154" uniqueCount="4661">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7156" uniqueCount="4663">
   <si>
     <t>Step</t>
   </si>
@@ -14062,6 +14062,12 @@
   </si>
   <si>
     <t>numeric</t>
+  </si>
+  <si>
+    <t>depressionSeverityScale</t>
+  </si>
+  <si>
+    <t>previous</t>
   </si>
 </sst>
 </file>
@@ -41608,10 +41614,10 @@
   <dimension ref="A1:AO13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="AF3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomRight" activeCell="AF20" sqref="AF20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -41637,7 +41643,7 @@
     <col min="27" max="27" width="15.5" customWidth="1" outlineLevel="1"/>
     <col min="28" max="28" width="9.5" customWidth="1" outlineLevel="1"/>
     <col min="29" max="31" width="4.5" customWidth="1" outlineLevel="1"/>
-    <col min="32" max="32" width="6.6640625" customWidth="1" outlineLevel="1"/>
+    <col min="32" max="32" width="255.83203125" bestFit="1" customWidth="1" outlineLevel="1"/>
     <col min="33" max="33" width="45.6640625" customWidth="1" outlineLevel="1"/>
     <col min="34" max="34" width="14.33203125" customWidth="1" outlineLevel="1"/>
     <col min="35" max="36" width="18.6640625" customWidth="1" outlineLevel="1"/>
@@ -42450,14 +42456,19 @@
       <c r="V13" s="52"/>
       <c r="W13" t="str">
         <f t="shared" si="0"/>
-        <v>Missing</v>
+        <v>Found</v>
       </c>
       <c r="Y13" t="s">
         <v>279</v>
       </c>
-      <c r="Z13" s="51"/>
+      <c r="Z13" t="s">
+        <v>4661</v>
+      </c>
       <c r="AA13" s="30"/>
       <c r="AB13" s="30"/>
+      <c r="AF13" t="s">
+        <v>4662</v>
+      </c>
       <c r="AH13" s="30"/>
     </row>
   </sheetData>
@@ -42828,7 +42839,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Cross-reference between questions, add calculation features documentation to README
</commit_message>
<xml_diff>
--- a/metadata_example.xlsx
+++ b/metadata_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajalodora/clinical-content-tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14BC38EA-7550-3B48-B1DA-75F007BC5D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A6D80C-691E-3F43-8D44-D7B0AAE64052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="1700" windowWidth="33600" windowHeight="19320" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4760" yWindow="1140" windowWidth="31080" windowHeight="19620" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Registration Workflow" sheetId="1" state="hidden" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7156" uniqueCount="4663">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7158" uniqueCount="4664">
   <si>
     <t>Step</t>
   </si>
@@ -14067,14 +14067,17 @@
     <t>depressionSeverityScale</t>
   </si>
   <si>
-    <t>previous</t>
+    <t>ref:speakingSlowly</t>
+  </si>
+  <si>
+    <t>latest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -14209,6 +14212,12 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFECC48D"/>
+      <name val="Menlo"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="18">
@@ -14348,7 +14357,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -14483,6 +14492,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -41614,10 +41624,10 @@
   <dimension ref="A1:AO13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="AF3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AF20" sqref="AF20"/>
+      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -42334,12 +42344,17 @@
       <c r="V11" s="52"/>
       <c r="W11" t="str">
         <f t="shared" si="0"/>
-        <v>Missing</v>
+        <v>Found</v>
       </c>
       <c r="Y11" t="s">
         <v>279</v>
       </c>
-      <c r="Z11" s="51"/>
+      <c r="Z11" s="60" t="s">
+        <v>312</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>4662</v>
+      </c>
       <c r="AK11" t="s">
         <v>280</v>
       </c>
@@ -42467,7 +42482,7 @@
       <c r="AA13" s="30"/>
       <c r="AB13" s="30"/>
       <c r="AF13" t="s">
-        <v>4662</v>
+        <v>4663</v>
       </c>
       <c r="AH13" s="30"/>
     </row>

</xml_diff>

<commit_message>
(fix) Add min/max bounds to numeric fields
</commit_message>
<xml_diff>
--- a/metadata_example.xlsx
+++ b/metadata_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajalodora/clinical-content-tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0179AD61-39C3-E74F-9C7B-39EF11853D68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D4292D4-DE2C-5440-AC75-CA741AAE31CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="33600" windowHeight="19320" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9520" yWindow="-19620" windowWidth="31080" windowHeight="19620" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Registration Workflow" sheetId="1" state="hidden" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7154" uniqueCount="4661">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7158" uniqueCount="4664">
   <si>
     <t>Step</t>
   </si>
@@ -14062,13 +14062,22 @@
   </si>
   <si>
     <t>numeric</t>
+  </si>
+  <si>
+    <t>depressionSeverityScale</t>
+  </si>
+  <si>
+    <t>ref:speakingSlowly</t>
+  </si>
+  <si>
+    <t>latest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -14203,6 +14212,12 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFECC48D"/>
+      <name val="Menlo"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="18">
@@ -14342,7 +14357,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -14468,6 +14483,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -41608,10 +41624,10 @@
   <dimension ref="A1:AO13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="AC3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomRight" activeCell="AE12" sqref="AE12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -41636,8 +41652,10 @@
     <col min="26" max="26" width="18.6640625" customWidth="1" outlineLevel="1"/>
     <col min="27" max="27" width="15.5" customWidth="1" outlineLevel="1"/>
     <col min="28" max="28" width="9.5" customWidth="1" outlineLevel="1"/>
-    <col min="29" max="31" width="4.5" customWidth="1" outlineLevel="1"/>
-    <col min="32" max="32" width="6.6640625" customWidth="1" outlineLevel="1"/>
+    <col min="29" max="29" width="9.6640625" customWidth="1" outlineLevel="1"/>
+    <col min="30" max="30" width="14.6640625" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="12.33203125" customWidth="1" outlineLevel="1"/>
+    <col min="32" max="32" width="255.83203125" bestFit="1" customWidth="1" outlineLevel="1"/>
     <col min="33" max="33" width="45.6640625" customWidth="1" outlineLevel="1"/>
     <col min="34" max="34" width="14.33203125" customWidth="1" outlineLevel="1"/>
     <col min="35" max="36" width="18.6640625" customWidth="1" outlineLevel="1"/>
@@ -41649,28 +41667,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K1" s="55" t="s">
+      <c r="K1" s="56" t="s">
         <v>229</v>
       </c>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="57"/>
-      <c r="Q1" s="55" t="s">
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="56" t="s">
         <v>230</v>
       </c>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="V1" s="57"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="58"/>
       <c r="W1" s="46"/>
-      <c r="X1" s="58" t="s">
+      <c r="X1" s="59" t="s">
         <v>231</v>
       </c>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="56"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
     </row>
     <row r="2" spans="1:41" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -42328,12 +42346,17 @@
       <c r="V11" s="52"/>
       <c r="W11" t="str">
         <f t="shared" si="0"/>
-        <v>Missing</v>
+        <v>Found</v>
       </c>
       <c r="Y11" t="s">
         <v>279</v>
       </c>
-      <c r="Z11" s="51"/>
+      <c r="Z11" s="55" t="s">
+        <v>312</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>4662</v>
+      </c>
       <c r="AK11" t="s">
         <v>280</v>
       </c>
@@ -42390,7 +42413,7 @@
       </c>
       <c r="AB12" s="30"/>
       <c r="AD12">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AE12" s="39">
         <v>27</v>
@@ -42450,14 +42473,19 @@
       <c r="V13" s="52"/>
       <c r="W13" t="str">
         <f t="shared" si="0"/>
-        <v>Missing</v>
+        <v>Found</v>
       </c>
       <c r="Y13" t="s">
         <v>279</v>
       </c>
-      <c r="Z13" s="51"/>
+      <c r="Z13" t="s">
+        <v>4661</v>
+      </c>
       <c r="AA13" s="30"/>
       <c r="AB13" s="30"/>
+      <c r="AF13" t="s">
+        <v>4663</v>
+      </c>
       <c r="AH13" s="30"/>
     </row>
   </sheetData>
@@ -42533,22 +42561,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G1" s="55" t="s">
+      <c r="G1" s="56" t="s">
         <v>229</v>
       </c>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="55" t="s">
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="56" t="s">
         <v>230</v>
       </c>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57"/>
+      <c r="R1" s="58"/>
       <c r="S1" s="46"/>
       <c r="T1" s="41" t="s">
         <v>231</v>
@@ -42828,7 +42856,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>